<commit_message>
update stored procedure names
</commit_message>
<xml_diff>
--- a/public/games/hello-kitty-island-adventure/hello-kitty-island-adventure_tables.xlsx
+++ b/public/games/hello-kitty-island-adventure/hello-kitty-island-adventure_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubChelsea\Achievement-Vault\public\games\hello-kitty-island-adventure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05490B45-5C80-4998-8CE7-0EAD0E3E77DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D37B985-CEC4-4505-9CCE-4D38EE729F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5115" yWindow="2520" windowWidth="21600" windowHeight="12525" activeTab="3" xr2:uid="{EDF2BE8D-03F7-4EE0-AD1E-08AEE49FD7D6}"/>
+    <workbookView xWindow="3735" yWindow="1545" windowWidth="19530" windowHeight="13200" activeTab="3" xr2:uid="{EDF2BE8D-03F7-4EE0-AD1E-08AEE49FD7D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="7" r:id="rId1"/>
@@ -1034,9 +1034,6 @@
     <t>Fruits, Bakery, Fancy</t>
   </si>
   <si>
-    <t>Candied Banana Coffee, Strawberry Shortcake, Beignets with Pineapple Dip, Mama's Apple Pie, Fruity Cheesecake, Strawberry Cheesecake</t>
-  </si>
-  <si>
     <t xml:space="preserve">Any Baked Goods, Any Themed Gift, Banana Shake, Strawberry Shake, Apple Ice Cream, Strawberry Ice Cream, Fruity Cloud, Designer Island Doll, Strawberry Soda, Apple Soda, Spinip Alfredo Pizza, Fruit Pizza, Strawberry, Pineapple, Apple, </t>
   </si>
   <si>
@@ -1281,6 +1278,9 @@
   </si>
   <si>
     <t>Default Order</t>
+  </si>
+  <si>
+    <t>Misc. Dessert</t>
   </si>
 </sst>
 </file>
@@ -1744,7 +1744,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB14B9A7-32BD-458D-A5F7-E49A0C0475BC}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1756,7 +1758,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B1" t="s">
         <v>324</v>
@@ -1788,10 +1790,10 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
+        <v>413</v>
+      </c>
+      <c r="F2" t="s">
         <v>331</v>
-      </c>
-      <c r="F2" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1802,16 +1804,16 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D3" t="s">
         <v>86</v>
       </c>
       <c r="E3" t="s">
+        <v>333</v>
+      </c>
+      <c r="F3" t="s">
         <v>334</v>
-      </c>
-      <c r="F3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1822,16 +1824,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>340</v>
+      </c>
+      <c r="D4" t="s">
         <v>341</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>342</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>343</v>
-      </c>
-      <c r="F4" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1842,16 +1844,16 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D5" t="s">
         <v>345</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>346</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>347</v>
-      </c>
-      <c r="F5" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1865,13 +1867,13 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
+        <v>348</v>
+      </c>
+      <c r="E6" t="s">
         <v>349</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>350</v>
-      </c>
-      <c r="F6" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1882,16 +1884,16 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
+        <v>351</v>
+      </c>
+      <c r="D7" t="s">
         <v>352</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>353</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>354</v>
-      </c>
-      <c r="F7" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1902,16 +1904,16 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
+        <v>355</v>
+      </c>
+      <c r="D8" t="s">
         <v>356</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>357</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>358</v>
-      </c>
-      <c r="F8" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1925,13 +1927,13 @@
         <v>325</v>
       </c>
       <c r="D9" t="s">
+        <v>359</v>
+      </c>
+      <c r="E9" t="s">
         <v>360</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>361</v>
-      </c>
-      <c r="F9" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1942,16 +1944,16 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
+        <v>362</v>
+      </c>
+      <c r="D10" t="s">
         <v>363</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>365</v>
+      </c>
+      <c r="F10" t="s">
         <v>364</v>
-      </c>
-      <c r="E10" t="s">
-        <v>366</v>
-      </c>
-      <c r="F10" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1965,13 +1967,13 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
+        <v>366</v>
+      </c>
+      <c r="E11" t="s">
         <v>367</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>368</v>
-      </c>
-      <c r="F11" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1982,16 +1984,16 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D12" t="s">
         <v>56</v>
       </c>
       <c r="E12" t="s">
+        <v>370</v>
+      </c>
+      <c r="F12" t="s">
         <v>371</v>
-      </c>
-      <c r="F12" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2002,16 +2004,16 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
+        <v>372</v>
+      </c>
+      <c r="D13" t="s">
         <v>373</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>374</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>375</v>
-      </c>
-      <c r="F13" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2022,16 +2024,16 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
+        <v>376</v>
+      </c>
+      <c r="D14" t="s">
         <v>377</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>378</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>379</v>
-      </c>
-      <c r="F14" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2042,16 +2044,16 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
+        <v>380</v>
+      </c>
+      <c r="D15" t="s">
         <v>381</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>382</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>383</v>
-      </c>
-      <c r="F15" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2062,16 +2064,16 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
+        <v>384</v>
+      </c>
+      <c r="D16" t="s">
         <v>385</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>386</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>387</v>
-      </c>
-      <c r="F16" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2079,19 +2081,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C17" t="s">
+        <v>388</v>
+      </c>
+      <c r="D17" t="s">
         <v>389</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>390</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>391</v>
-      </c>
-      <c r="F17" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2099,19 +2101,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C18" t="s">
+        <v>392</v>
+      </c>
+      <c r="D18" t="s">
         <v>393</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>394</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>395</v>
-      </c>
-      <c r="F18" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2119,19 +2121,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C19" t="s">
+        <v>396</v>
+      </c>
+      <c r="D19" t="s">
         <v>397</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>398</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>399</v>
-      </c>
-      <c r="F19" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2139,19 +2141,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C20" t="s">
+        <v>400</v>
+      </c>
+      <c r="D20" t="s">
         <v>401</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>402</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>403</v>
-      </c>
-      <c r="F20" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2159,19 +2161,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C21" t="s">
+        <v>404</v>
+      </c>
+      <c r="D21" t="s">
         <v>405</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>406</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>407</v>
-      </c>
-      <c r="F21" t="s">
-        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -2188,7 +2190,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A2" sqref="A2:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2202,7 +2204,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B1" t="s">
         <v>16</v>
@@ -2672,7 +2674,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4FD85B-59D8-4D29-B4AF-8683988B5507}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:G57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2684,7 +2688,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B1" t="s">
         <v>220</v>
@@ -2702,7 +2706,7 @@
         <v>91</v>
       </c>
       <c r="G1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2726,7 +2730,7 @@
         <v>95</v>
       </c>
       <c r="G2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2750,7 +2754,7 @@
         <v>98</v>
       </c>
       <c r="G3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2774,7 +2778,7 @@
         <v>95</v>
       </c>
       <c r="G4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2798,7 +2802,7 @@
         <v>95</v>
       </c>
       <c r="G5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2822,7 +2826,7 @@
         <v>105</v>
       </c>
       <c r="G6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2846,7 +2850,7 @@
         <v>107</v>
       </c>
       <c r="G7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2870,7 +2874,7 @@
         <v>110</v>
       </c>
       <c r="G8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2894,7 +2898,7 @@
         <v>95</v>
       </c>
       <c r="G9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2918,7 +2922,7 @@
         <v>98</v>
       </c>
       <c r="G10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2942,7 +2946,7 @@
         <v>95</v>
       </c>
       <c r="G11" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2966,7 +2970,7 @@
         <v>95</v>
       </c>
       <c r="G12" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2990,7 +2994,7 @@
         <v>98</v>
       </c>
       <c r="G13" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3014,7 +3018,7 @@
         <v>95</v>
       </c>
       <c r="G14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3038,7 +3042,7 @@
         <v>95</v>
       </c>
       <c r="G15" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -3062,7 +3066,7 @@
         <v>98</v>
       </c>
       <c r="G16" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -3086,7 +3090,7 @@
         <v>107</v>
       </c>
       <c r="G17" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -3110,7 +3114,7 @@
         <v>98</v>
       </c>
       <c r="G18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -3134,7 +3138,7 @@
         <v>95</v>
       </c>
       <c r="G19" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -3158,7 +3162,7 @@
         <v>95</v>
       </c>
       <c r="G20" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -3182,7 +3186,7 @@
         <v>98</v>
       </c>
       <c r="G21" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -3206,7 +3210,7 @@
         <v>95</v>
       </c>
       <c r="G22" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -3230,7 +3234,7 @@
         <v>95</v>
       </c>
       <c r="G23" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -3254,7 +3258,7 @@
         <v>144</v>
       </c>
       <c r="G24" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -3278,7 +3282,7 @@
         <v>107</v>
       </c>
       <c r="G25" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -3302,7 +3306,7 @@
         <v>149</v>
       </c>
       <c r="G26" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -3326,7 +3330,7 @@
         <v>110</v>
       </c>
       <c r="G27" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -3350,7 +3354,7 @@
         <v>95</v>
       </c>
       <c r="G28" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -3374,7 +3378,7 @@
         <v>107</v>
       </c>
       <c r="G29" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -3398,7 +3402,7 @@
         <v>98</v>
       </c>
       <c r="G30" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -3422,7 +3426,7 @@
         <v>159</v>
       </c>
       <c r="G31" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -3446,7 +3450,7 @@
         <v>95</v>
       </c>
       <c r="G32" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -3470,7 +3474,7 @@
         <v>110</v>
       </c>
       <c r="G33" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -3494,7 +3498,7 @@
         <v>95</v>
       </c>
       <c r="G34" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -3518,7 +3522,7 @@
         <v>95</v>
       </c>
       <c r="G35" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -3542,7 +3546,7 @@
         <v>169</v>
       </c>
       <c r="G36" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -3566,7 +3570,7 @@
         <v>107</v>
       </c>
       <c r="G37" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3590,7 +3594,7 @@
         <v>107</v>
       </c>
       <c r="G38" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3614,7 +3618,7 @@
         <v>176</v>
       </c>
       <c r="G39" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3638,7 +3642,7 @@
         <v>179</v>
       </c>
       <c r="G40" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -3662,7 +3666,7 @@
         <v>181</v>
       </c>
       <c r="G41" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3686,7 +3690,7 @@
         <v>181</v>
       </c>
       <c r="G42" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -3710,7 +3714,7 @@
         <v>186</v>
       </c>
       <c r="G43" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3734,7 +3738,7 @@
         <v>189</v>
       </c>
       <c r="G44" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -3758,7 +3762,7 @@
         <v>110</v>
       </c>
       <c r="G45" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3782,7 +3786,7 @@
         <v>159</v>
       </c>
       <c r="G46" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -3806,7 +3810,7 @@
         <v>95</v>
       </c>
       <c r="G47" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -3830,7 +3834,7 @@
         <v>110</v>
       </c>
       <c r="G48" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3854,7 +3858,7 @@
         <v>98</v>
       </c>
       <c r="G49" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -3878,7 +3882,7 @@
         <v>204</v>
       </c>
       <c r="G50" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -3902,7 +3906,7 @@
         <v>95</v>
       </c>
       <c r="G51" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3926,7 +3930,7 @@
         <v>95</v>
       </c>
       <c r="G52" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3950,7 +3954,7 @@
         <v>95</v>
       </c>
       <c r="G53" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -3974,7 +3978,7 @@
         <v>95</v>
       </c>
       <c r="G54" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -3998,7 +4002,7 @@
         <v>95</v>
       </c>
       <c r="G55" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -4022,7 +4026,7 @@
         <v>107</v>
       </c>
       <c r="G56" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -4046,7 +4050,7 @@
         <v>98</v>
       </c>
       <c r="G57" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>
@@ -4061,7 +4065,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E0F9F24-98FF-4930-82DA-5BF13106EE36}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4075,7 +4081,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B1" t="s">
         <v>220</v>
@@ -4093,7 +4099,7 @@
         <v>91</v>
       </c>
       <c r="G1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4117,7 +4123,7 @@
         <v>95</v>
       </c>
       <c r="G2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4141,7 +4147,7 @@
         <v>228</v>
       </c>
       <c r="G3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4165,7 +4171,7 @@
         <v>107</v>
       </c>
       <c r="G4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4189,7 +4195,7 @@
         <v>186</v>
       </c>
       <c r="G5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -4213,7 +4219,7 @@
         <v>228</v>
       </c>
       <c r="G6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -4237,7 +4243,7 @@
         <v>98</v>
       </c>
       <c r="G7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -4261,7 +4267,7 @@
         <v>181</v>
       </c>
       <c r="G8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -4285,7 +4291,7 @@
         <v>98</v>
       </c>
       <c r="G9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4309,7 +4315,7 @@
         <v>95</v>
       </c>
       <c r="G10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -4333,7 +4339,7 @@
         <v>186</v>
       </c>
       <c r="G11" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -4357,7 +4363,7 @@
         <v>95</v>
       </c>
       <c r="G12" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -4381,7 +4387,7 @@
         <v>98</v>
       </c>
       <c r="G13" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -4405,7 +4411,7 @@
         <v>95</v>
       </c>
       <c r="G14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4429,7 +4435,7 @@
         <v>181</v>
       </c>
       <c r="G15" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -4453,7 +4459,7 @@
         <v>95</v>
       </c>
       <c r="G16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -4477,7 +4483,7 @@
         <v>95</v>
       </c>
       <c r="G17" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -4501,7 +4507,7 @@
         <v>186</v>
       </c>
       <c r="G18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -4525,7 +4531,7 @@
         <v>98</v>
       </c>
       <c r="G19" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -4549,7 +4555,7 @@
         <v>144</v>
       </c>
       <c r="G20" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -4573,7 +4579,7 @@
         <v>95</v>
       </c>
       <c r="G21" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -4597,7 +4603,7 @@
         <v>204</v>
       </c>
       <c r="G22" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -4621,7 +4627,7 @@
         <v>110</v>
       </c>
       <c r="G23" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -4645,7 +4651,7 @@
         <v>110</v>
       </c>
       <c r="G24" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -4669,7 +4675,7 @@
         <v>95</v>
       </c>
       <c r="G25" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -4693,7 +4699,7 @@
         <v>107</v>
       </c>
       <c r="G26" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -4717,7 +4723,7 @@
         <v>95</v>
       </c>
       <c r="G27" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -4741,7 +4747,7 @@
         <v>110</v>
       </c>
       <c r="G28" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -4765,7 +4771,7 @@
         <v>179</v>
       </c>
       <c r="G29" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -4789,7 +4795,7 @@
         <v>95</v>
       </c>
       <c r="G30" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -4813,7 +4819,7 @@
         <v>110</v>
       </c>
       <c r="G31" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -4837,7 +4843,7 @@
         <v>228</v>
       </c>
       <c r="G32" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -4861,7 +4867,7 @@
         <v>98</v>
       </c>
       <c r="G33" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -4885,7 +4891,7 @@
         <v>98</v>
       </c>
       <c r="G34" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -4909,7 +4915,7 @@
         <v>95</v>
       </c>
       <c r="G35" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -4933,7 +4939,7 @@
         <v>95</v>
       </c>
       <c r="G36" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -4957,7 +4963,7 @@
         <v>95</v>
       </c>
       <c r="G37" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -4981,7 +4987,7 @@
         <v>176</v>
       </c>
       <c r="G38" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -5005,7 +5011,7 @@
         <v>95</v>
       </c>
       <c r="G39" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -5029,7 +5035,7 @@
         <v>95</v>
       </c>
       <c r="G40" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -5053,7 +5059,7 @@
         <v>228</v>
       </c>
       <c r="G41" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -5077,7 +5083,7 @@
         <v>186</v>
       </c>
       <c r="G42" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -5101,7 +5107,7 @@
         <v>95</v>
       </c>
       <c r="G43" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -5125,7 +5131,7 @@
         <v>110</v>
       </c>
       <c r="G44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -5149,7 +5155,7 @@
         <v>105</v>
       </c>
       <c r="G45" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -5173,7 +5179,7 @@
         <v>95</v>
       </c>
       <c r="G46" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -5197,7 +5203,7 @@
         <v>95</v>
       </c>
       <c r="G47" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -5221,7 +5227,7 @@
         <v>308</v>
       </c>
       <c r="G48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -5245,7 +5251,7 @@
         <v>98</v>
       </c>
       <c r="G49" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -5269,7 +5275,7 @@
         <v>95</v>
       </c>
       <c r="G50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -5293,7 +5299,7 @@
         <v>312</v>
       </c>
       <c r="G51" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -5317,7 +5323,7 @@
         <v>95</v>
       </c>
       <c r="G52" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -5341,7 +5347,7 @@
         <v>95</v>
       </c>
       <c r="G53" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -5389,7 +5395,7 @@
         <v>98</v>
       </c>
       <c r="G55" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -5413,7 +5419,7 @@
         <v>110</v>
       </c>
       <c r="G56" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -5437,7 +5443,7 @@
         <v>95</v>
       </c>
       <c r="G57" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>